<commit_message>
charset for Chinese and files re-organization
</commit_message>
<xml_diff>
--- a/excel_file/437.xlsx
+++ b/excel_file/437.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t/>
   </si>
@@ -25,18 +25,33 @@
     <t xml:space="preserve"> ZSF</t>
   </si>
   <si>
+    <t>&amp;#20320;&amp;#23478;</t>
+  </si>
+  <si>
     <t>&amp;#21608;&amp;#39034;&amp;#39118;</t>
   </si>
   <si>
+    <t>&amp;#21621;&amp;#21621;</t>
+  </si>
+  <si>
     <t>&amp;#24352;&amp;#24191;&amp;#24609;</t>
   </si>
   <si>
     <t>&amp;#27888;&amp;#22269;</t>
   </si>
   <si>
+    <t>000000</t>
+  </si>
+  <si>
+    <t>000000\</t>
+  </si>
+  <si>
     <t>12345</t>
   </si>
   <si>
+    <t>123456</t>
+  </si>
+  <si>
     <t>1234567890</t>
   </si>
   <si>
@@ -65,6 +80,12 @@
   </si>
   <si>
     <t>周顺风\</t>
+  </si>
+  <si>
+    <t>呵呵</t>
+  </si>
+  <si>
+    <t>呵呵\</t>
   </si>
   <si>
     <t>回家</t>
@@ -95,6 +116,9 @@
     <t>留校</t>
   </si>
   <si>
+    <t>碧荷</t>
+  </si>
+  <si>
     <t>联系电话</t>
   </si>
   <si>
@@ -102,6 +126,9 @@
   </si>
   <si>
     <t>闫仕伟</t>
+  </si>
+  <si>
+    <t>齐哥的家</t>
   </si>
 </sst>
 </file>
@@ -707,7 +734,7 @@
   <sheetData>
     <row customFormat="1" ht="22.5" customHeight="1" s="2" r="1" spans="1:5">
       <c s="19" r="A1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c s="20" r="B1" t="s"/>
       <c s="20" r="C1" t="s"/>
@@ -717,19 +744,19 @@
     </row>
     <row customFormat="1" ht="18.75" customHeight="1" s="3" r="2" spans="1:5">
       <c s="6" r="A2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c s="6" r="B2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c s="6" r="C2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c s="6" r="D2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c s="6" r="E2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c s="7" r="F2" t="s"/>
     </row>
@@ -738,22 +765,22 @@
       <c s="6" r="B3" t="s"/>
       <c s="6" r="C3" t="s"/>
       <c s="6" r="D3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c s="6" r="E3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c s="7" r="F3" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="4" spans="1:5">
       <c s="8" r="A4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c s="9" r="B4" t="n">
         <v>13570348561</v>
       </c>
       <c s="9" r="C4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c s="9" r="D4" t="s"/>
       <c s="9" r="E4" t="s"/>
@@ -761,13 +788,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="5" spans="1:5">
       <c s="9" r="A5" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c s="9" r="B5" t="n">
         <v>13235698899</v>
       </c>
       <c s="9" r="C5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c s="9" r="D5" t="s"/>
       <c s="9" r="E5" t="s"/>
@@ -775,13 +802,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="6" spans="1:5">
       <c s="9" r="A6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c s="9" r="B6" t="n">
         <v>13576478952</v>
       </c>
       <c s="9" r="C6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c s="9" r="D6" t="s"/>
       <c s="9" r="E6" t="s"/>
@@ -789,13 +816,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="7" spans="1:5">
       <c s="11" r="A7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c s="12" r="B7" t="n">
         <v>13589547231</v>
       </c>
       <c s="13" r="C7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c s="9" r="D7" t="s"/>
       <c s="9" r="E7" t="s"/>
@@ -803,13 +830,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="8" spans="1:5">
       <c s="11" r="A8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c s="14" r="B8" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c s="9" r="C8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="13" r="D8" t="s"/>
       <c s="9" r="E8" t="s"/>
@@ -817,13 +844,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="9" spans="1:5">
       <c s="11" r="A9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c s="15" r="B9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c s="9" r="C9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="13" r="D9" t="s"/>
       <c s="9" r="E9" t="s"/>
@@ -834,28 +861,28 @@
         <v>1</v>
       </c>
       <c s="15" r="B10" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c s="9" r="C10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="13" r="D10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c s="9" r="E10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c s="10" r="F10" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="11" spans="1:5">
       <c s="8" r="A11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c s="9" r="B11" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c s="9" r="C11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="9" r="D11" t="s"/>
       <c s="9" r="E11" t="s"/>
@@ -863,13 +890,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="12" spans="1:5">
       <c s="11" r="A12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c s="13" r="B12" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c s="13" r="C12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="13" r="D12" t="s"/>
       <c s="13" r="E12" t="s"/>
@@ -877,13 +904,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="13" spans="1:5">
       <c s="11" r="A13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c s="13" r="B13" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c s="13" r="C13" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="13" r="D13" t="s"/>
       <c s="13" r="E13" t="s"/>
@@ -891,13 +918,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="14" spans="1:5">
       <c s="11" r="A14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="13" r="B14" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c s="13" r="C14" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="13" r="D14" t="s"/>
       <c s="13" r="E14" t="s"/>
@@ -905,13 +932,13 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="15" spans="1:5">
       <c s="11" r="A15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="13" r="B15" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c s="13" r="C15" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="13" r="D15" t="s"/>
       <c s="13" r="E15" t="s"/>
@@ -919,45 +946,45 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="16" spans="1:5">
       <c s="13" r="A16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="13" r="B16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c s="13" r="C16" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c s="13" r="D16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c s="13" r="E16" t="s"/>
       <c s="10" r="F16" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="17" spans="1:5">
       <c s="13" r="A17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="13" r="B17" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c s="13" r="C17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c s="13" r="D17" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c s="13" r="E17" t="s"/>
       <c s="10" r="F17" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="18" spans="1:5">
       <c s="13" r="A18" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c s="13" r="B18" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c s="13" r="C18" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c s="13" r="D18" t="s"/>
       <c s="13" r="E18" t="s"/>
@@ -965,177 +992,267 @@
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="19" spans="1:5">
       <c s="13" r="A19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="13" r="B19" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c s="13" r="C19" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c s="13" r="D19" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c s="13" r="E19" t="s"/>
       <c s="10" r="F19" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="20" spans="1:5">
       <c s="11" r="A20" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="13" r="B20" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c s="13" r="C20" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c s="13" r="D20" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c s="13" r="E20" t="s"/>
       <c s="10" r="F20" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="21" spans="1:5">
       <c s="11" r="A21" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="13" r="B21" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c s="13" r="C21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c s="13" r="D21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c s="13" r="E21" t="s"/>
       <c s="10" r="F21" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="22" spans="1:5">
       <c s="11" r="A22" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="13" r="B22" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c s="13" r="C22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c s="13" r="D22" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c s="13" r="E22" t="s"/>
       <c s="10" r="F22" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="23" spans="1:5">
-      <c s="11" r="A23" t="s"/>
-      <c s="13" r="B23" t="s"/>
-      <c s="13" r="C23" t="s"/>
+      <c s="11" r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c s="13" r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c s="13" r="C23" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D23" t="s"/>
       <c s="13" r="E23" t="s"/>
       <c s="10" r="F23" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="24" spans="1:5">
-      <c s="11" r="A24" t="s"/>
-      <c s="13" r="B24" t="s"/>
-      <c s="13" r="C24" t="s"/>
-      <c s="13" r="D24" t="s"/>
+      <c s="11" r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c s="13" r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c s="13" r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c s="13" r="D24" t="s">
+        <v>2</v>
+      </c>
       <c s="13" r="E24" t="s"/>
       <c s="10" r="F24" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="25" spans="1:5">
-      <c s="11" r="A25" t="s"/>
-      <c s="13" r="B25" t="s"/>
-      <c s="13" r="C25" t="s"/>
+      <c s="11" r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c s="13" r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c s="13" r="C25" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D25" t="s"/>
       <c s="13" r="E25" t="s"/>
       <c s="10" r="F25" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="26" spans="1:5">
-      <c s="11" r="A26" t="s"/>
-      <c s="13" r="B26" t="s"/>
-      <c s="13" r="C26" t="s"/>
-      <c s="13" r="D26" t="s"/>
+      <c s="11" r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c s="13" r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c s="13" r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c s="13" r="D26" t="s">
+        <v>2</v>
+      </c>
       <c s="13" r="E26" t="s"/>
       <c s="10" r="F26" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="27" spans="1:5">
-      <c s="11" r="A27" t="s"/>
-      <c s="13" r="B27" t="s"/>
-      <c s="13" r="C27" t="s"/>
+      <c s="11" r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c s="13" r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c s="13" r="C27" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D27" t="s"/>
       <c s="13" r="E27" t="s"/>
       <c s="10" r="F27" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="28" spans="1:5">
-      <c s="11" r="A28" t="s"/>
-      <c s="13" r="B28" t="s"/>
-      <c s="13" r="C28" t="s"/>
+      <c s="11" r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c s="13" r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c s="13" r="C28" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D28" t="s"/>
       <c s="13" r="E28" t="s"/>
       <c s="10" r="F28" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="29" spans="1:5">
-      <c s="11" r="A29" t="s"/>
-      <c s="15" r="B29" t="s"/>
-      <c s="13" r="C29" t="s"/>
+      <c s="11" r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c s="15" r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c s="13" r="C29" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D29" t="s"/>
       <c s="13" r="E29" t="s"/>
       <c s="10" r="F29" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="30" spans="1:5">
-      <c s="11" r="A30" t="s"/>
-      <c s="15" r="B30" t="s"/>
-      <c s="13" r="C30" t="s"/>
+      <c s="11" r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c s="15" r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c s="13" r="C30" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D30" t="s"/>
       <c s="13" r="E30" t="s"/>
       <c s="10" r="F30" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="31" spans="1:5">
-      <c s="11" r="A31" t="s"/>
-      <c s="15" r="B31" t="s"/>
-      <c s="13" r="C31" t="s"/>
+      <c s="11" r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c s="15" r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c s="13" r="C31" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D31" t="s"/>
       <c s="13" r="E31" t="s"/>
       <c s="10" r="F31" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="32" spans="1:5">
-      <c s="11" r="A32" t="s"/>
-      <c s="15" r="B32" t="s"/>
-      <c s="13" r="C32" t="s"/>
+      <c s="11" r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c s="15" r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c s="13" r="C32" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D32" t="s"/>
       <c s="13" r="E32" t="s"/>
       <c s="10" r="F32" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="33" spans="1:5">
-      <c s="13" r="A33" t="s"/>
-      <c s="15" r="B33" t="s"/>
-      <c s="13" r="C33" t="s"/>
+      <c s="13" r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c s="15" r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c s="13" r="C33" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D33" t="s"/>
       <c s="13" r="E33" t="s"/>
       <c s="10" r="F33" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="34" spans="1:5">
-      <c s="11" r="A34" t="s"/>
-      <c s="15" r="B34" t="s"/>
-      <c s="13" r="C34" t="s"/>
+      <c s="11" r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c s="15" r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c s="13" r="C34" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D34" t="s"/>
       <c s="13" r="E34" t="s"/>
       <c s="10" r="F34" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="35" spans="1:5">
-      <c s="11" r="A35" t="s"/>
-      <c s="15" r="B35" t="s"/>
-      <c s="13" r="C35" t="s"/>
+      <c s="11" r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c s="15" r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c s="13" r="C35" t="s">
+        <v>15</v>
+      </c>
       <c s="13" r="D35" t="s"/>
       <c s="13" r="E35" t="s"/>
       <c s="10" r="F35" t="s"/>
     </row>
     <row customFormat="1" ht="14.25" customHeight="1" s="4" r="36" spans="1:5">
-      <c s="11" r="A36" t="s"/>
-      <c s="15" r="B36" t="s"/>
-      <c s="13" r="C36" t="s"/>
-      <c s="13" r="D36" t="s"/>
+      <c s="11" r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c s="15" r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c s="13" r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c s="13" r="D36" t="s">
+        <v>36</v>
+      </c>
       <c s="13" r="E36" t="s"/>
       <c s="10" r="F36" t="s"/>
     </row>
@@ -1202,7 +1319,7 @@
     </row>
     <row customHeight="1" r="45" ht="13.5" spans="1:5">
       <c s="21" r="A45" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c s="22" r="B45" t="s"/>
       <c s="22" r="C45" t="s"/>

</xml_diff>